<commit_message>
Prefill the biosample name grid in the template.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_identity_QC_v5_1_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_identity_QC_v5_1_0.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SampleIdentityQC" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Info" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Index" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="QcContainer" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Info" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Index" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="451">
   <si>
     <t xml:space="preserve">Sample Identity QC Template</t>
   </si>
@@ -77,58 +78,133 @@
     <t xml:space="preserve">Source Container Coord</t>
   </si>
   <si>
+    <t xml:space="preserve">Destination Container Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destination Container Coord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destination Container Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destination Container Kind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume Used (uL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QC Date (YYYY-MM-DD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workflow Action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample Identity QC template instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample Identity QC template adjust the volume of the sample and provide the QC container for the QC values to be store in Freezeman once the processing is done.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the "Keep Source Coord for Destination" is set to "Yes" the QC container coordinates will be set to the source coordinates.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details on fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample name of the source of the QC. This is used for validation purpose to confirm the expected sample matches the container location.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique barcode of the container holding the source sample.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coordinate of the source sample within the container. Using the alphanumerical coordinates names (e.g. A01).</t>
+  </si>
+  <si>
     <t xml:space="preserve">QC Container Barcode</t>
   </si>
   <si>
+    <t xml:space="preserve">Unique barcode of the container holding the QCed sample.</t>
+  </si>
+  <si>
     <t xml:space="preserve">QC Container Coord</t>
   </si>
   <si>
+    <t xml:space="preserve">Coordinate of the QCed sample within the container. Using the alphanumerical coordinates names (e.g. A01).</t>
+  </si>
+  <si>
     <t xml:space="preserve">QC Container Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Name of the destination container. The container barcode will be used as name if none is provided.</t>
+  </si>
+  <si>
     <t xml:space="preserve">QC Container Kind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume Used (uL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QC Date (YYYY-MM-DD)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Workflow Action</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample Identity QC template instructions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample Identity QC template adjust the volume of the sample and provide the QC container for the QC values to be store in Freezeman once the processing is done.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the "Keep Source Coord for Destination" is set to "Yes" the QC container coordinates will be set to the source coordinates.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Details on fields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample name of the source of the QC. This is used for validation purpose to confirm the expected sample matches the container location.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique barcode of the container holding the source sample.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordinate of the source sample within the container. Using the alphanumerical coordinates names (e.g. A01).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique barcode of the container holding the QCed sample.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordinate of the QCed sample within the container. Using the alphanumerical coordinates names (e.g. A01).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of the destination container. The container barcode will be used as name if none is provided.</t>
   </si>
   <si>
     <t xml:space="preserve">Kind of the destination container.</t>
@@ -1445,7 +1521,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1460,8 +1536,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F9D4"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFAFD095"/>
-        <bgColor rgb="FF92D050"/>
+        <bgColor rgb="FFB4C7DC"/>
       </patternFill>
     </fill>
   </fills>
@@ -1632,7 +1720,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1761,6 +1849,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1785,7 +1889,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1818,11 +1922,11 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFAFD095"/>
+      <rgbColor rgb="FFB4C7DC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFF6F9D4"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -1840,7 +1944,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -1872,13 +1976,13 @@
   </sheetPr>
   <dimension ref="A1:Z892"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.21"/>
@@ -8667,20 +8771,222 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:M1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:V1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.41015625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -8730,7 +9036,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -8756,7 +9062,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -8804,8 +9110,8 @@
       <c r="V5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="32" t="s">
-        <v>19</v>
+      <c r="A6" s="36" t="s">
+        <v>40</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -8828,8 +9134,8 @@
       <c r="V6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="33"/>
-      <c r="C7" s="34"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -8851,13 +9157,13 @@
       <c r="V7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="34"/>
+      <c r="B8" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="38"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -8879,13 +9185,13 @@
       <c r="V8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="37"/>
+      <c r="B9" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="41"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -8907,13 +9213,13 @@
       <c r="V9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="37"/>
+      <c r="B10" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="41"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -8935,13 +9241,13 @@
       <c r="V10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="37"/>
+      <c r="A11" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="41"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -8963,13 +9269,13 @@
       <c r="V11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="37"/>
+      <c r="A12" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="41"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -8991,13 +9297,13 @@
       <c r="V12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="37"/>
+      <c r="A13" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="41"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -9019,13 +9325,13 @@
       <c r="V13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="37"/>
+      <c r="A14" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="41"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -9047,13 +9353,13 @@
       <c r="V14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="37"/>
+      <c r="B15" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="41"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -9075,13 +9381,13 @@
       <c r="V15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="37"/>
+      <c r="B16" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="41"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -9103,13 +9409,13 @@
       <c r="V16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="37"/>
+      <c r="B17" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="41"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -9131,11 +9437,11 @@
       <c r="V17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="36" t="s">
-        <v>30</v>
+      <c r="B18" s="40" t="s">
+        <v>55</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -9765,7 +10071,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -9776,7 +10082,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.47"/>
@@ -9787,17 +10093,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>32</v>
+      <c r="A1" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>57</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>15</v>
@@ -9807,2523 +10113,2523 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>35</v>
+      <c r="A2" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>60</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>40</v>
+      <c r="A3" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>65</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>44</v>
+      <c r="A4" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>69</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>47</v>
+      <c r="A5" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>72</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>50</v>
+      <c r="A6" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>75</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="39" t="s">
-        <v>52</v>
+      <c r="A7" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>77</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="39" t="s">
-        <v>54</v>
+      <c r="A8" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>79</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="39" t="s">
-        <v>56</v>
+      <c r="A9" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>81</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="39" t="s">
-        <v>57</v>
+      <c r="A10" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>82</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>59</v>
+      <c r="A11" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>84</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="39" t="s">
-        <v>61</v>
+      <c r="A12" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>86</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="39" t="s">
-        <v>63</v>
+      <c r="A13" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>88</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="39" t="s">
-        <v>39</v>
-      </c>
       <c r="C14" s="3" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="39" t="s">
-        <v>58</v>
+      <c r="A15" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="43" t="s">
+        <v>83</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39" t="s">
+      <c r="C26" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="B30" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="39" t="s">
+      <c r="C38" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="B45" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="B46" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="B48" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="43" t="s">
+        <v>160</v>
+      </c>
+      <c r="B49" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="39" t="s">
+      <c r="C50" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="B52" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="B53" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="B54" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="B55" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="B56" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="B57" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="B58" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="B59" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B60" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="B61" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="B62" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39" t="s">
+      <c r="C62" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="B63" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="B64" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="B65" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="B66" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="B67" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B68" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="B69" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="B70" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="B71" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="B72" s="43" t="s">
+        <v>188</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="B73" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B74" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="C74" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="B75" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="B76" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="B77" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="B78" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="B79" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="B80" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="43" t="s">
+        <v>194</v>
+      </c>
+      <c r="B81" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B82" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="B83" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="B84" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="B85" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" s="43" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="B23" s="39" t="s">
+      <c r="C86" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="43" t="s">
+        <v>188</v>
+      </c>
+      <c r="B87" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="B88" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="43" t="s">
+        <v>200</v>
+      </c>
+      <c r="B89" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A90" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="B24" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="39" t="s">
-        <v>99</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="39" t="s">
-        <v>100</v>
-      </c>
-      <c r="B31" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="B32" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="B33" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="39" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="B37" s="39" t="s">
-        <v>110</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="B38" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="B39" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="B40" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="B41" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="C42" s="3" t="s">
+      <c r="B90" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A91" s="43" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="B44" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="B45" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="B46" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="B47" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="B48" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="39" t="s">
+      <c r="B91" s="43" t="s">
+        <v>160</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A92" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="B49" s="39" t="s">
-        <v>136</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="B50" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="B51" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="B52" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="B53" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="B54" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="B55" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="39" t="s">
-        <v>140</v>
-      </c>
-      <c r="B56" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="B57" s="39" t="s">
-        <v>142</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="B59" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="B60" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="B61" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="39" t="s">
-        <v>142</v>
-      </c>
-      <c r="B62" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="B63" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="B64" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="B65" s="39" t="s">
-        <v>100</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B66" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="B67" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="B68" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="B69" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="B70" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="B71" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="C71" s="3" t="s">
+      <c r="B92" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A93" s="43" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="B72" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="B73" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="B74" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="B75" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="B76" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="B77" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="B78" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="B79" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="39" t="s">
-        <v>168</v>
-      </c>
-      <c r="B80" s="39" t="s">
-        <v>140</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="39" t="s">
-        <v>169</v>
-      </c>
-      <c r="B81" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="B82" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="B83" s="39" t="s">
-        <v>168</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="B84" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="B85" s="39" t="s">
+      <c r="B93" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A94" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="C85" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="B86" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="B87" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="B88" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="B89" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="B90" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="B91" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="39" t="s">
-        <v>110</v>
-      </c>
-      <c r="B92" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="39" t="s">
-        <v>136</v>
-      </c>
-      <c r="B93" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="B94" s="39" t="s">
-        <v>165</v>
+      <c r="B94" s="43" t="s">
+        <v>190</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>181</v>
+        <v>206</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="B95" s="39" t="s">
-        <v>169</v>
+      <c r="A95" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="B95" s="43" t="s">
+        <v>194</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="B96" s="39" t="s">
-        <v>175</v>
+      <c r="A96" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="B96" s="43" t="s">
+        <v>200</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="39" t="s">
-        <v>184</v>
-      </c>
-      <c r="B97" s="39" t="s">
-        <v>184</v>
+      <c r="A97" s="43" t="s">
+        <v>209</v>
+      </c>
+      <c r="B97" s="43" t="s">
+        <v>209</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>185</v>
+        <v>210</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C98" s="3" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C99" s="3" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C100" s="3" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C101" s="3" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C102" s="3" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C103" s="3" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C104" s="3" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C105" s="3" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C106" s="3" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C107" s="3" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C108" s="3" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C109" s="3" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C110" s="3" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C111" s="3" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C112" s="3" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C113" s="3" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C114" s="3" t="s">
-        <v>190</v>
+        <v>215</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C115" s="3" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C116" s="3" t="s">
-        <v>192</v>
+        <v>217</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C117" s="3" t="s">
-        <v>193</v>
+        <v>218</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C118" s="3" t="s">
-        <v>194</v>
+        <v>219</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C119" s="3" t="s">
-        <v>195</v>
+        <v>220</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C120" s="3" t="s">
-        <v>196</v>
+        <v>221</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C121" s="3" t="s">
-        <v>197</v>
+        <v>222</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C122" s="3" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C123" s="3" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C124" s="3" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C125" s="3" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C126" s="3" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C127" s="3" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C128" s="3" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C129" s="3" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C130" s="3" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C131" s="3" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C132" s="3" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C133" s="3" t="s">
-        <v>166</v>
+        <v>191</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C134" s="3" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C135" s="3" t="s">
-        <v>199</v>
+        <v>224</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C136" s="3" t="s">
-        <v>200</v>
+        <v>225</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C137" s="3" t="s">
-        <v>201</v>
+        <v>226</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C138" s="3" t="s">
-        <v>202</v>
+        <v>227</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C139" s="3" t="s">
-        <v>203</v>
+        <v>228</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C140" s="3" t="s">
-        <v>204</v>
+        <v>229</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C141" s="3" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C142" s="3" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C143" s="3" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C144" s="3" t="s">
-        <v>208</v>
+        <v>233</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C145" s="3" t="s">
-        <v>209</v>
+        <v>234</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C146" s="3" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C147" s="3" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C148" s="3" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C149" s="3" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C150" s="3" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C151" s="3" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C152" s="3" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C153" s="3" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C154" s="3" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C155" s="3" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C156" s="3" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C157" s="3" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C158" s="3" t="s">
-        <v>210</v>
+        <v>235</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C159" s="3" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C160" s="3" t="s">
-        <v>212</v>
+        <v>237</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C161" s="3" t="s">
-        <v>213</v>
+        <v>238</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C162" s="3" t="s">
-        <v>214</v>
+        <v>239</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C163" s="3" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C164" s="3" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C165" s="3" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C166" s="3" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C167" s="3" t="s">
-        <v>219</v>
+        <v>244</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C168" s="3" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C169" s="3" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C170" s="3" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C171" s="3" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C172" s="3" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C173" s="3" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C174" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C175" s="3" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C176" s="3" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C177" s="3" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C178" s="3" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C179" s="3" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C180" s="3" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C181" s="3" t="s">
-        <v>184</v>
+        <v>209</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C182" s="3" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C183" s="3" t="s">
-        <v>223</v>
+        <v>248</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C184" s="3" t="s">
-        <v>224</v>
+        <v>249</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C185" s="3" t="s">
-        <v>225</v>
+        <v>250</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C186" s="3" t="s">
-        <v>226</v>
+        <v>251</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C187" s="3" t="s">
-        <v>227</v>
+        <v>252</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C188" s="3" t="s">
-        <v>228</v>
+        <v>253</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C189" s="3" t="s">
-        <v>229</v>
+        <v>254</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C190" s="3" t="s">
-        <v>230</v>
+        <v>255</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C191" s="3" t="s">
-        <v>231</v>
+        <v>256</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C192" s="3" t="s">
-        <v>232</v>
+        <v>257</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C193" s="3" t="s">
-        <v>233</v>
+        <v>258</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C194" s="3" t="s">
-        <v>234</v>
+        <v>259</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C195" s="3" t="s">
-        <v>235</v>
+        <v>260</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C196" s="3" t="s">
-        <v>236</v>
+        <v>261</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C197" s="3" t="s">
-        <v>237</v>
+        <v>262</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C198" s="3" t="s">
-        <v>238</v>
+        <v>263</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C199" s="3" t="s">
-        <v>239</v>
+        <v>264</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C200" s="3" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C201" s="3" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C202" s="3" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C203" s="3" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C204" s="3" t="s">
-        <v>244</v>
+        <v>269</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C205" s="3" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C206" s="3" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C207" s="3" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C208" s="3" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C209" s="3" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C210" s="3" t="s">
-        <v>250</v>
+        <v>275</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C211" s="3" t="s">
-        <v>251</v>
+        <v>276</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C212" s="3" t="s">
-        <v>252</v>
+        <v>277</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C213" s="3" t="s">
-        <v>253</v>
+        <v>278</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C214" s="3" t="s">
-        <v>254</v>
+        <v>279</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C215" s="3" t="s">
-        <v>255</v>
+        <v>280</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C216" s="3" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C217" s="3" t="s">
-        <v>257</v>
+        <v>282</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C218" s="3" t="s">
-        <v>258</v>
+        <v>283</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C219" s="3" t="s">
-        <v>259</v>
+        <v>284</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C220" s="3" t="s">
-        <v>260</v>
+        <v>285</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C221" s="3" t="s">
-        <v>261</v>
+        <v>286</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C222" s="3" t="s">
-        <v>262</v>
+        <v>287</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C223" s="3" t="s">
-        <v>263</v>
+        <v>288</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C224" s="3" t="s">
-        <v>264</v>
+        <v>289</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C225" s="3" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C226" s="3" t="s">
-        <v>266</v>
+        <v>291</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C227" s="3" t="s">
-        <v>267</v>
+        <v>292</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C228" s="3" t="s">
-        <v>268</v>
+        <v>293</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C229" s="3" t="s">
-        <v>269</v>
+        <v>294</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C230" s="3" t="s">
-        <v>270</v>
+        <v>295</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C231" s="3" t="s">
-        <v>271</v>
+        <v>296</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C232" s="3" t="s">
-        <v>272</v>
+        <v>297</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C233" s="3" t="s">
-        <v>273</v>
+        <v>298</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C234" s="3" t="s">
-        <v>274</v>
+        <v>299</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C235" s="3" t="s">
-        <v>275</v>
+        <v>300</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C236" s="3" t="s">
-        <v>276</v>
+        <v>301</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C237" s="3" t="s">
-        <v>277</v>
+        <v>302</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C238" s="3" t="s">
-        <v>278</v>
+        <v>303</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C239" s="3" t="s">
-        <v>279</v>
+        <v>304</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C240" s="3" t="s">
-        <v>280</v>
+        <v>305</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C241" s="3" t="s">
-        <v>281</v>
+        <v>306</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C242" s="3" t="s">
-        <v>282</v>
+        <v>307</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C243" s="3" t="s">
-        <v>283</v>
+        <v>308</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C244" s="3" t="s">
-        <v>284</v>
+        <v>309</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C245" s="3" t="s">
-        <v>285</v>
+        <v>310</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C246" s="3" t="s">
-        <v>286</v>
+        <v>311</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C247" s="3" t="s">
-        <v>287</v>
+        <v>312</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C248" s="3" t="s">
-        <v>288</v>
+        <v>313</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C249" s="3" t="s">
-        <v>289</v>
+        <v>314</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C250" s="3" t="s">
-        <v>290</v>
+        <v>315</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C251" s="3" t="s">
-        <v>291</v>
+        <v>316</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C252" s="3" t="s">
-        <v>292</v>
+        <v>317</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C253" s="3" t="s">
-        <v>293</v>
+        <v>318</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C254" s="3" t="s">
-        <v>294</v>
+        <v>319</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C255" s="3" t="s">
-        <v>295</v>
+        <v>320</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C256" s="3" t="s">
-        <v>296</v>
+        <v>321</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C257" s="3" t="s">
-        <v>297</v>
+        <v>322</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C258" s="3" t="s">
-        <v>298</v>
+        <v>323</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C259" s="3" t="s">
-        <v>299</v>
+        <v>324</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C260" s="3" t="s">
-        <v>300</v>
+        <v>325</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C261" s="3" t="s">
-        <v>301</v>
+        <v>326</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C262" s="3" t="s">
-        <v>302</v>
+        <v>327</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C263" s="3" t="s">
-        <v>303</v>
+        <v>328</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C264" s="3" t="s">
-        <v>304</v>
+        <v>329</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C265" s="3" t="s">
-        <v>305</v>
+        <v>330</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C266" s="3" t="s">
-        <v>306</v>
+        <v>331</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C267" s="3" t="s">
-        <v>307</v>
+        <v>332</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C268" s="3" t="s">
-        <v>308</v>
+        <v>333</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C269" s="3" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C270" s="3" t="s">
-        <v>310</v>
+        <v>335</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C271" s="3" t="s">
-        <v>311</v>
+        <v>336</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C272" s="3" t="s">
-        <v>312</v>
+        <v>337</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C273" s="3" t="s">
-        <v>313</v>
+        <v>338</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C274" s="3" t="s">
-        <v>314</v>
+        <v>339</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C275" s="3" t="s">
-        <v>315</v>
+        <v>340</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C276" s="3" t="s">
-        <v>316</v>
+        <v>341</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C277" s="3" t="s">
-        <v>317</v>
+        <v>342</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C278" s="3" t="s">
-        <v>318</v>
+        <v>343</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C279" s="3" t="s">
-        <v>319</v>
+        <v>344</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C280" s="3" t="s">
-        <v>320</v>
+        <v>345</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C281" s="3" t="s">
-        <v>321</v>
+        <v>346</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C282" s="3" t="s">
-        <v>322</v>
+        <v>347</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C283" s="3" t="s">
-        <v>323</v>
+        <v>348</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C284" s="3" t="s">
-        <v>324</v>
+        <v>349</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C285" s="3" t="s">
-        <v>325</v>
+        <v>350</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C286" s="3" t="s">
-        <v>326</v>
+        <v>351</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C287" s="3" t="s">
-        <v>327</v>
+        <v>352</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C288" s="3" t="s">
-        <v>328</v>
+        <v>353</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C289" s="3" t="s">
-        <v>329</v>
+        <v>354</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C290" s="3" t="s">
-        <v>330</v>
+        <v>355</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C291" s="3" t="s">
-        <v>331</v>
+        <v>356</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C292" s="3" t="s">
-        <v>332</v>
+        <v>357</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C293" s="3" t="s">
-        <v>333</v>
+        <v>358</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C294" s="3" t="s">
-        <v>334</v>
+        <v>359</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C295" s="3" t="s">
-        <v>335</v>
+        <v>360</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C296" s="3" t="s">
-        <v>336</v>
+        <v>361</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C297" s="3" t="s">
-        <v>337</v>
+        <v>362</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C298" s="3" t="s">
-        <v>338</v>
+        <v>363</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C299" s="3" t="s">
-        <v>339</v>
+        <v>364</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C300" s="3" t="s">
-        <v>340</v>
+        <v>365</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C301" s="3" t="s">
-        <v>341</v>
+        <v>366</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C302" s="3" t="s">
-        <v>342</v>
+        <v>367</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C303" s="3" t="s">
-        <v>343</v>
+        <v>368</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C304" s="3" t="s">
-        <v>344</v>
+        <v>369</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C305" s="3" t="s">
-        <v>345</v>
+        <v>370</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C306" s="3" t="s">
-        <v>346</v>
+        <v>371</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C307" s="3" t="s">
-        <v>347</v>
+        <v>372</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C308" s="3" t="s">
-        <v>348</v>
+        <v>373</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C309" s="3" t="s">
-        <v>349</v>
+        <v>374</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C310" s="3" t="s">
-        <v>350</v>
+        <v>375</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C311" s="3" t="s">
-        <v>351</v>
+        <v>376</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C312" s="3" t="s">
-        <v>352</v>
+        <v>377</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C313" s="3" t="s">
-        <v>353</v>
+        <v>378</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C314" s="3" t="s">
-        <v>354</v>
+        <v>379</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C315" s="3" t="s">
-        <v>355</v>
+        <v>380</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C316" s="3" t="s">
-        <v>356</v>
+        <v>381</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C317" s="3" t="s">
-        <v>357</v>
+        <v>382</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C318" s="3" t="s">
-        <v>358</v>
+        <v>383</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C319" s="3" t="s">
-        <v>359</v>
+        <v>384</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C320" s="3" t="s">
-        <v>360</v>
+        <v>385</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C321" s="3" t="s">
-        <v>361</v>
+        <v>386</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C322" s="3" t="s">
-        <v>362</v>
+        <v>387</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C323" s="3" t="s">
-        <v>363</v>
+        <v>388</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C324" s="3" t="s">
-        <v>364</v>
+        <v>389</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C325" s="3" t="s">
-        <v>365</v>
+        <v>390</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C326" s="3" t="s">
-        <v>366</v>
+        <v>391</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C327" s="3" t="s">
-        <v>367</v>
+        <v>392</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C328" s="3" t="s">
-        <v>368</v>
+        <v>393</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C329" s="3" t="s">
-        <v>369</v>
+        <v>394</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C330" s="3" t="s">
-        <v>370</v>
+        <v>395</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C331" s="3" t="s">
-        <v>371</v>
+        <v>396</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C332" s="3" t="s">
-        <v>372</v>
+        <v>397</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C333" s="3" t="s">
-        <v>373</v>
+        <v>398</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C334" s="3" t="s">
-        <v>374</v>
+        <v>399</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C335" s="3" t="s">
-        <v>375</v>
+        <v>400</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C336" s="3" t="s">
-        <v>376</v>
+        <v>401</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C337" s="3" t="s">
-        <v>377</v>
+        <v>402</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C338" s="3" t="s">
-        <v>378</v>
+        <v>403</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C339" s="3" t="s">
-        <v>379</v>
+        <v>404</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C340" s="3" t="s">
-        <v>380</v>
+        <v>405</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C341" s="3" t="s">
-        <v>381</v>
+        <v>406</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C342" s="3" t="s">
-        <v>382</v>
+        <v>407</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C343" s="3" t="s">
-        <v>383</v>
+        <v>408</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C344" s="3" t="s">
-        <v>384</v>
+        <v>409</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C345" s="3" t="s">
-        <v>385</v>
+        <v>410</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C346" s="3" t="s">
-        <v>386</v>
+        <v>411</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C347" s="3" t="s">
-        <v>387</v>
+        <v>412</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C348" s="3" t="s">
-        <v>388</v>
+        <v>413</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C349" s="3" t="s">
-        <v>389</v>
+        <v>414</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C350" s="3" t="s">
-        <v>390</v>
+        <v>415</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C351" s="3" t="s">
-        <v>391</v>
+        <v>416</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C352" s="3" t="s">
-        <v>392</v>
+        <v>417</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C353" s="3" t="s">
-        <v>393</v>
+        <v>418</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C354" s="3" t="s">
-        <v>394</v>
+        <v>419</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C355" s="3" t="s">
-        <v>395</v>
+        <v>420</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C356" s="3" t="s">
-        <v>396</v>
+        <v>421</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C357" s="3" t="s">
-        <v>397</v>
+        <v>422</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C358" s="3" t="s">
-        <v>398</v>
+        <v>423</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C359" s="3" t="s">
-        <v>399</v>
+        <v>424</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C360" s="3" t="s">
-        <v>400</v>
+        <v>425</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C361" s="3" t="s">
-        <v>401</v>
+        <v>426</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C362" s="3" t="s">
-        <v>402</v>
+        <v>427</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C363" s="3" t="s">
-        <v>403</v>
+        <v>428</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C364" s="3" t="s">
-        <v>404</v>
+        <v>429</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C365" s="3" t="s">
-        <v>405</v>
+        <v>430</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C366" s="3" t="s">
-        <v>406</v>
+        <v>431</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C367" s="3" t="s">
-        <v>407</v>
+        <v>432</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C368" s="3" t="s">
-        <v>408</v>
+        <v>433</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C369" s="3" t="s">
-        <v>409</v>
+        <v>434</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C370" s="3" t="s">
-        <v>410</v>
+        <v>435</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C371" s="3" t="s">
-        <v>411</v>
+        <v>436</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C372" s="3" t="s">
-        <v>412</v>
+        <v>437</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C373" s="3" t="s">
-        <v>413</v>
+        <v>438</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C374" s="3" t="s">
-        <v>414</v>
+        <v>439</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C375" s="3" t="s">
-        <v>415</v>
+        <v>440</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C376" s="3" t="s">
-        <v>416</v>
+        <v>441</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C377" s="3" t="s">
-        <v>417</v>
+        <v>442</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C378" s="3" t="s">
-        <v>418</v>
+        <v>443</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C379" s="3" t="s">
-        <v>419</v>
+        <v>444</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C380" s="3" t="s">
-        <v>420</v>
+        <v>445</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C381" s="3" t="s">
-        <v>421</v>
+        <v>446</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C382" s="3" t="s">
-        <v>422</v>
+        <v>447</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C383" s="3" t="s">
-        <v>423</v>
+        <v>448</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C384" s="3" t="s">
-        <v>424</v>
+        <v>449</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C385" s="3" t="s">
-        <v>425</v>
+        <v>450</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Fixed a couple of issues. Returns errors if submit without placement.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_identity_QC_v5_1_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_identity_QC_v5_1_0.xlsx
@@ -93,40 +93,40 @@
     <t xml:space="preserve">Coord</t>
   </si>
   <si>
-    <t xml:space="preserve">01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12</t>
+    <t xml:space="preserve">col 01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col 02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col 03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col 04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col 05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col 06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col 07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col 08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col 09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col 12</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -1842,7 +1842,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.21"/>
@@ -6297,7 +6297,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
@@ -6499,7 +6499,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.33"/>
   </cols>
@@ -7519,7 +7519,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.47"/>

</xml_diff>

<commit_message>
Fix column names in template QcContainer tab.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_identity_QC_v5_1_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_identity_QC_v5_1_0.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="437">
   <si>
     <t xml:space="preserve">Sample Identity QC Template</t>
   </si>
@@ -93,40 +93,40 @@
     <t xml:space="preserve">Coord</t>
   </si>
   <si>
-    <t xml:space="preserve">col 01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">col 02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">col 03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">col 04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">col 05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">col 06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">col 07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">col 08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">col 09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">col 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">col 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">col 12</t>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -1628,7 +1628,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1709,6 +1709,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1717,11 +1725,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1842,7 +1846,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.50390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.21"/>
@@ -6291,192 +6295,233 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="1" style="20" width="10.42"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
-        <v>12</v>
-      </c>
+      <c r="A1" s="0"/>
       <c r="B1" s="21" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
+        <v>12</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
+        <v>25</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
+        <v>26</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
+        <v>27</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
+        <v>28</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
+        <v>29</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
+        <v>30</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -6499,7 +6544,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.35546875" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.33"/>
   </cols>
@@ -6628,7 +6673,7 @@
       <c r="V5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="25" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="3"/>
@@ -6652,8 +6697,8 @@
       <c r="V6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -6675,13 +6720,13 @@
       <c r="V7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="26"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -6703,13 +6748,13 @@
       <c r="V8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="29"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -6731,13 +6776,13 @@
       <c r="V9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="29"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -6759,13 +6804,13 @@
       <c r="V10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="29"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -6787,13 +6832,13 @@
       <c r="V11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="29"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -6815,13 +6860,13 @@
       <c r="V12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="29"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -6843,13 +6888,13 @@
       <c r="V13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="29"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -6871,10 +6916,10 @@
       <c r="V14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="29" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="3"/>
@@ -7519,7 +7564,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.50390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.47"/>
@@ -7530,10 +7575,10 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>45</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -7548,10 +7593,10 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>48</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -7566,10 +7611,10 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="32" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -7582,10 +7627,10 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="32" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -7597,10 +7642,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="32" t="s">
         <v>58</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -7612,10 +7657,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="32" t="s">
         <v>61</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -7623,10 +7668,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="32" t="s">
         <v>63</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -7634,10 +7679,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="32" t="s">
         <v>65</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -7645,10 +7690,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="32" t="s">
         <v>67</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -7656,10 +7701,10 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="32" t="s">
         <v>68</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -7667,10 +7712,10 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="32" t="s">
         <v>70</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -7678,10 +7723,10 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="32" t="s">
         <v>72</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -7689,10 +7734,10 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="32" t="s">
         <v>74</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -7700,10 +7745,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="32" t="s">
         <v>51</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -7711,10 +7756,10 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="32" t="s">
         <v>69</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -7722,10 +7767,10 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="32" t="s">
         <v>80</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -7733,10 +7778,10 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="32" t="s">
         <v>83</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -7744,10 +7789,10 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="32" t="s">
         <v>85</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -7755,10 +7800,10 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="32" t="s">
         <v>87</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -7766,10 +7811,10 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="32" t="s">
         <v>90</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -7777,10 +7822,10 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="32" t="s">
         <v>93</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -7788,10 +7833,10 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="32" t="s">
         <v>96</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -7799,10 +7844,10 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="32" t="s">
         <v>99</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -7810,10 +7855,10 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="32" t="s">
         <v>102</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -7821,10 +7866,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="32" t="s">
         <v>105</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -7832,10 +7877,10 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="32" t="s">
         <v>54</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -7843,10 +7888,10 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="32" t="s">
         <v>71</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -7854,10 +7899,10 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="32" t="s">
         <v>89</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -7865,10 +7910,10 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="32" t="s">
         <v>107</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -7876,10 +7921,10 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="32" t="s">
         <v>110</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -7887,10 +7932,10 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="32" t="s">
         <v>112</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -7898,10 +7943,10 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="32" t="s">
         <v>114</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -7909,10 +7954,10 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="32" t="s">
         <v>116</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -7920,10 +7965,10 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="32" t="s">
         <v>117</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -7931,10 +7976,10 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="32" t="s">
         <v>118</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -7942,10 +7987,10 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="32" t="s">
         <v>119</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -7953,10 +7998,10 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="32" t="s">
         <v>121</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -7964,10 +8009,10 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="32" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -7975,10 +8020,10 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="32" t="s">
         <v>73</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -7986,10 +8031,10 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="32" t="s">
         <v>92</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -7997,10 +8042,10 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="32" t="s">
         <v>108</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -8008,10 +8053,10 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="B42" s="31" t="s">
+      <c r="B42" s="32" t="s">
         <v>120</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -8019,10 +8064,10 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="32" t="s">
         <v>131</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -8030,10 +8075,10 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="B44" s="31" t="s">
+      <c r="B44" s="32" t="s">
         <v>133</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -8041,10 +8086,10 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="32" t="s">
         <v>135</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -8052,10 +8097,10 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="B46" s="31" t="s">
+      <c r="B46" s="32" t="s">
         <v>138</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -8063,10 +8108,10 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="B47" s="31" t="s">
+      <c r="B47" s="32" t="s">
         <v>141</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -8074,10 +8119,10 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="B48" s="31" t="s">
+      <c r="B48" s="32" t="s">
         <v>144</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -8085,10 +8130,10 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="32" t="s">
         <v>147</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -8096,10 +8141,10 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="32" t="s">
         <v>60</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -8107,10 +8152,10 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="B51" s="31" t="s">
+      <c r="B51" s="32" t="s">
         <v>75</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -8118,10 +8163,10 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="B52" s="31" t="s">
+      <c r="B52" s="32" t="s">
         <v>95</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -8129,10 +8174,10 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="31" t="s">
+      <c r="A53" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="B53" s="31" t="s">
+      <c r="B53" s="32" t="s">
         <v>109</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -8140,10 +8185,10 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="B54" s="31" t="s">
+      <c r="B54" s="32" t="s">
         <v>122</v>
       </c>
       <c r="C54" s="3" t="s">
@@ -8151,10 +8196,10 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="B55" s="31" t="s">
+      <c r="B55" s="32" t="s">
         <v>137</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -8162,10 +8207,10 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="31" t="s">
+      <c r="A56" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="B56" s="31" t="s">
+      <c r="B56" s="32" t="s">
         <v>149</v>
       </c>
       <c r="C56" s="3" t="s">
@@ -8173,10 +8218,10 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="31" t="s">
+      <c r="A57" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="B57" s="31" t="s">
+      <c r="B57" s="32" t="s">
         <v>153</v>
       </c>
       <c r="C57" s="3" t="s">
@@ -8184,10 +8229,10 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="31" t="s">
+      <c r="A58" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B58" s="31" t="s">
+      <c r="B58" s="32" t="s">
         <v>154</v>
       </c>
       <c r="C58" s="3" t="s">
@@ -8195,10 +8240,10 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="31" t="s">
+      <c r="A59" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="B59" s="31" t="s">
+      <c r="B59" s="32" t="s">
         <v>155</v>
       </c>
       <c r="C59" s="3" t="s">
@@ -8206,10 +8251,10 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="31" t="s">
+      <c r="A60" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="B60" s="31" t="s">
+      <c r="B60" s="32" t="s">
         <v>156</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -8217,10 +8262,10 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="31" t="s">
+      <c r="A61" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="B61" s="31" t="s">
+      <c r="B61" s="32" t="s">
         <v>157</v>
       </c>
       <c r="C61" s="3" t="s">
@@ -8228,10 +8273,10 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="31" t="s">
+      <c r="A62" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="B62" s="31" t="s">
+      <c r="B62" s="32" t="s">
         <v>62</v>
       </c>
       <c r="C62" s="3" t="s">
@@ -8239,10 +8284,10 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="31" t="s">
+      <c r="A63" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="B63" s="31" t="s">
+      <c r="B63" s="32" t="s">
         <v>77</v>
       </c>
       <c r="C63" s="3" t="s">
@@ -8250,10 +8295,10 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="31" t="s">
+      <c r="A64" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="B64" s="31" t="s">
+      <c r="B64" s="32" t="s">
         <v>98</v>
       </c>
       <c r="C64" s="3" t="s">
@@ -8261,10 +8306,10 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="31" t="s">
+      <c r="A65" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="B65" s="31" t="s">
+      <c r="B65" s="32" t="s">
         <v>111</v>
       </c>
       <c r="C65" s="3" t="s">
@@ -8272,10 +8317,10 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="31" t="s">
+      <c r="A66" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="B66" s="31" t="s">
+      <c r="B66" s="32" t="s">
         <v>124</v>
       </c>
       <c r="C66" s="3" t="s">
@@ -8283,10 +8328,10 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="31" t="s">
+      <c r="A67" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="B67" s="31" t="s">
+      <c r="B67" s="32" t="s">
         <v>140</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -8294,10 +8339,10 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="31" t="s">
+      <c r="A68" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="B68" s="31" t="s">
+      <c r="B68" s="32" t="s">
         <v>150</v>
       </c>
       <c r="C68" s="3" t="s">
@@ -8305,10 +8350,10 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="31" t="s">
+      <c r="A69" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="B69" s="31" t="s">
+      <c r="B69" s="32" t="s">
         <v>159</v>
       </c>
       <c r="C69" s="3" t="s">
@@ -8316,10 +8361,10 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="31" t="s">
+      <c r="A70" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="B70" s="31" t="s">
+      <c r="B70" s="32" t="s">
         <v>169</v>
       </c>
       <c r="C70" s="3" t="s">
@@ -8327,10 +8372,10 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="31" t="s">
+      <c r="A71" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="B71" s="31" t="s">
+      <c r="B71" s="32" t="s">
         <v>171</v>
       </c>
       <c r="C71" s="3" t="s">
@@ -8338,10 +8383,10 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="31" t="s">
+      <c r="A72" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="B72" s="31" t="s">
+      <c r="B72" s="32" t="s">
         <v>174</v>
       </c>
       <c r="C72" s="3" t="s">
@@ -8349,10 +8394,10 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="31" t="s">
+      <c r="A73" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="B73" s="31" t="s">
+      <c r="B73" s="32" t="s">
         <v>177</v>
       </c>
       <c r="C73" s="3" t="s">
@@ -8360,10 +8405,10 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="31" t="s">
+      <c r="A74" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="B74" s="31" t="s">
+      <c r="B74" s="32" t="s">
         <v>64</v>
       </c>
       <c r="C74" s="3" t="s">
@@ -8371,10 +8416,10 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="31" t="s">
+      <c r="A75" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="B75" s="31" t="s">
+      <c r="B75" s="32" t="s">
         <v>79</v>
       </c>
       <c r="C75" s="3" t="s">
@@ -8382,10 +8427,10 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="31" t="s">
+      <c r="A76" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="B76" s="31" t="s">
+      <c r="B76" s="32" t="s">
         <v>101</v>
       </c>
       <c r="C76" s="3" t="s">
@@ -8393,10 +8438,10 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="31" t="s">
+      <c r="A77" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="B77" s="31" t="s">
+      <c r="B77" s="32" t="s">
         <v>113</v>
       </c>
       <c r="C77" s="3" t="s">
@@ -8404,10 +8449,10 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="31" t="s">
+      <c r="A78" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="B78" s="31" t="s">
+      <c r="B78" s="32" t="s">
         <v>126</v>
       </c>
       <c r="C78" s="3" t="s">
@@ -8415,10 +8460,10 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="31" t="s">
+      <c r="A79" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="B79" s="31" t="s">
+      <c r="B79" s="32" t="s">
         <v>143</v>
       </c>
       <c r="C79" s="3" t="s">
@@ -8426,10 +8471,10 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="31" t="s">
+      <c r="A80" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="B80" s="31" t="s">
+      <c r="B80" s="32" t="s">
         <v>151</v>
       </c>
       <c r="C80" s="3" t="s">
@@ -8437,10 +8482,10 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="31" t="s">
+      <c r="A81" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="B81" s="31" t="s">
+      <c r="B81" s="32" t="s">
         <v>161</v>
       </c>
       <c r="C81" s="3" t="s">
@@ -8448,10 +8493,10 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="31" t="s">
+      <c r="A82" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="B82" s="31" t="s">
+      <c r="B82" s="32" t="s">
         <v>173</v>
       </c>
       <c r="C82" s="3" t="s">
@@ -8459,10 +8504,10 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="31" t="s">
+      <c r="A83" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="B83" s="31" t="s">
+      <c r="B83" s="32" t="s">
         <v>179</v>
       </c>
       <c r="C83" s="3" t="s">
@@ -8470,10 +8515,10 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="31" t="s">
+      <c r="A84" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="B84" s="31" t="s">
+      <c r="B84" s="32" t="s">
         <v>181</v>
       </c>
       <c r="C84" s="3" t="s">
@@ -8481,10 +8526,10 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="31" t="s">
+      <c r="A85" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="B85" s="31" t="s">
+      <c r="B85" s="32" t="s">
         <v>182</v>
       </c>
       <c r="C85" s="3" t="s">
@@ -8492,10 +8537,10 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="31" t="s">
+      <c r="A86" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="B86" s="31" t="s">
+      <c r="B86" s="32" t="s">
         <v>66</v>
       </c>
       <c r="C86" s="3" t="s">
@@ -8503,10 +8548,10 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="31" t="s">
+      <c r="A87" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="B87" s="31" t="s">
+      <c r="B87" s="32" t="s">
         <v>82</v>
       </c>
       <c r="C87" s="3" t="s">
@@ -8514,10 +8559,10 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="31" t="s">
+      <c r="A88" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="B88" s="31" t="s">
+      <c r="B88" s="32" t="s">
         <v>104</v>
       </c>
       <c r="C88" s="3" t="s">
@@ -8525,10 +8570,10 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="31" t="s">
+      <c r="A89" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="B89" s="31" t="s">
+      <c r="B89" s="32" t="s">
         <v>115</v>
       </c>
       <c r="C89" s="3" t="s">
@@ -8536,10 +8581,10 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="31" t="s">
+      <c r="A90" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="B90" s="31" t="s">
+      <c r="B90" s="32" t="s">
         <v>128</v>
       </c>
       <c r="C90" s="3" t="s">
@@ -8547,10 +8592,10 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="31" t="s">
+      <c r="A91" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="B91" s="31" t="s">
+      <c r="B91" s="32" t="s">
         <v>146</v>
       </c>
       <c r="C91" s="3" t="s">
@@ -8558,10 +8603,10 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="31" t="s">
+      <c r="A92" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="B92" s="31" t="s">
+      <c r="B92" s="32" t="s">
         <v>152</v>
       </c>
       <c r="C92" s="3" t="s">
@@ -8569,10 +8614,10 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="31" t="s">
+      <c r="A93" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B93" s="31" t="s">
+      <c r="B93" s="32" t="s">
         <v>163</v>
       </c>
       <c r="C93" s="3" t="s">
@@ -8580,10 +8625,10 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="31" t="s">
+      <c r="A94" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="B94" s="31" t="s">
+      <c r="B94" s="32" t="s">
         <v>176</v>
       </c>
       <c r="C94" s="3" t="s">
@@ -8591,10 +8636,10 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="31" t="s">
+      <c r="A95" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="B95" s="31" t="s">
+      <c r="B95" s="32" t="s">
         <v>180</v>
       </c>
       <c r="C95" s="3" t="s">
@@ -8602,10 +8647,10 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="31" t="s">
+      <c r="A96" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="B96" s="31" t="s">
+      <c r="B96" s="32" t="s">
         <v>186</v>
       </c>
       <c r="C96" s="3" t="s">
@@ -8613,10 +8658,10 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="31" t="s">
+      <c r="A97" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="B97" s="31" t="s">
+      <c r="B97" s="32" t="s">
         <v>195</v>
       </c>
       <c r="C97" s="3" t="s">

</xml_diff>